<commit_message>
All POM Pages created
</commit_message>
<xml_diff>
--- a/websiteautomation/ExcelData/loginCredentials.xlsx
+++ b/websiteautomation/ExcelData/loginCredentials.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14790" windowHeight="6405" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="5790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O19"/>
+  <oleSize ref="A1:M17"/>
 </workbook>
 </file>
 
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +104,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,9 +187,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +239,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,11 +431,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -492,10 +529,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>